<commit_message>
Add Colorado Water Trust to Env Orgs map, issue #79
I also added to the instream flow reaches info doc.
</commit_message>
<xml_diff>
--- a/workflow/BasinEntities/Environment-Organizations/data/environment-orgs-data.xlsx
+++ b/workflow/BasinEntities/Environment-Organizations/data/environment-orgs-data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>Organization</t>
   </si>
@@ -190,12 +190,30 @@
   </si>
   <si>
     <t>https://warnercnr.colostate.edu/elc/</t>
+  </si>
+  <si>
+    <t>Colorado Water Trust</t>
+  </si>
+  <si>
+    <t>Restore flow to Colorado's rivers in need.</t>
+  </si>
+  <si>
+    <t>https://coloradowatertrust.org</t>
+  </si>
+  <si>
+    <t>The data are converted to GeoJSON using a TSTool command file.</t>
+  </si>
+  <si>
+    <t>Entitities that have offices outside the basin are shown at the outflow point from the basin.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -234,9 +252,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -518,15 +537,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -536,10 +567,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,226 +646,275 @@
       <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>-105.071971</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>40.596536999999998</v>
       </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3">
-        <v>-105.019846</v>
-      </c>
-      <c r="H3">
-        <v>40.556621999999997</v>
+        <v>50</v>
+      </c>
+      <c r="G3" s="2">
+        <v>-104.558258</v>
+      </c>
+      <c r="H3" s="2">
+        <v>40.407221999999997</v>
+      </c>
+      <c r="I3" s="2">
+        <v>-104.97686899999999</v>
+      </c>
+      <c r="J3" s="2">
+        <v>39.764792999999997</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="G4">
-        <v>-105.028807</v>
-      </c>
-      <c r="H4">
-        <v>40.562764999999999</v>
-      </c>
+      <c r="G4" s="2">
+        <v>-105.019846</v>
+      </c>
+      <c r="H4" s="2">
+        <v>40.556621999999997</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
       </c>
-      <c r="G5">
-        <v>-105.04508</v>
-      </c>
-      <c r="H5">
-        <v>40.574539000000001</v>
-      </c>
-      <c r="L5" t="s">
-        <v>35</v>
-      </c>
+      <c r="G5" s="2">
+        <v>-105.028807</v>
+      </c>
+      <c r="H5" s="2">
+        <v>40.562764999999999</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
       </c>
-      <c r="G6">
-        <v>-105.112968</v>
-      </c>
-      <c r="H6">
-        <v>40.402273000000001</v>
-      </c>
+      <c r="G6" s="2">
+        <v>-105.04508</v>
+      </c>
+      <c r="H6" s="2">
+        <v>40.574539000000001</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
       <c r="L6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="G7">
-        <v>-105.076746</v>
-      </c>
-      <c r="H7">
-        <v>40.595180999999997</v>
-      </c>
+      <c r="G7" s="2">
+        <v>-105.112968</v>
+      </c>
+      <c r="H7" s="2">
+        <v>40.402273000000001</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
       <c r="L7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8">
-        <v>-105.25764100000001</v>
-      </c>
-      <c r="H8">
-        <v>40.805090999999997</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-105.076746</v>
+      </c>
+      <c r="H8" s="2">
+        <v>40.595180999999997</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="L8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="2">
+        <v>-105.25764100000001</v>
+      </c>
+      <c r="H9" s="2">
+        <v>40.805090999999997</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>40</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>7</v>
       </c>
-      <c r="G9">
+      <c r="G10" s="2">
         <v>-105.254758</v>
       </c>
-      <c r="H9">
+      <c r="H10" s="2">
         <v>40.804403000000001</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L10" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E7" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E6" r:id="rId4"/>
-    <hyperlink ref="E5" r:id="rId5"/>
-    <hyperlink ref="E9" r:id="rId6"/>
-    <hyperlink ref="K9" r:id="rId7"/>
-    <hyperlink ref="K8" r:id="rId8"/>
-    <hyperlink ref="E8" r:id="rId9"/>
+    <hyperlink ref="E8" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E7" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E10" r:id="rId6"/>
+    <hyperlink ref="K10" r:id="rId7"/>
+    <hyperlink ref="K9" r:id="rId8"/>
+    <hyperlink ref="E9" r:id="rId9"/>
+    <hyperlink ref="E3" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>